<commit_message>
added simulation for strain 1h2 on remote
</commit_message>
<xml_diff>
--- a/DFT_absorption/absorption_energies.xlsx
+++ b/DFT_absorption/absorption_energies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edoardocabiati/Desktop/Cose_brutte_PoliMI/V_anno/II_semestre/Molecular_Modeling_for_Materials/MMoM_project/MMoM_project/DFT_absorption/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADE8749-CABC-E54C-AE61-6B141CAD8D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA11684-E055-A441-9245-495DAAE20551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2640" yWindow="1100" windowWidth="25220" windowHeight="17440" activeTab="1" xr2:uid="{BDE33051-051D-5449-958A-46A8E86A2B7A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
   <si>
     <t>number of hydrogen
  moleclues</t>
@@ -290,6 +290,9 @@
   <si>
     <t>Interlayer 
 expansion [c/a]</t>
+  </si>
+  <si>
+    <t>Strain energy [Ry]</t>
   </si>
 </sst>
 </file>
@@ -1398,7 +1401,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1589,6 +1592,13 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -6543,14 +6553,14 @@
   <dimension ref="A2:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
     <col min="4" max="5" width="16.1640625" customWidth="1"/>
     <col min="6" max="6" width="16.83203125" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
@@ -6926,6 +6936,24 @@
       <c r="I13" s="77">
         <f t="shared" si="3"/>
         <v>0.280501533966108</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="2:6" ht="41" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="91" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="89">
+        <v>1</v>
+      </c>
+      <c r="C19" s="90">
+        <f>E5+287.15029323</f>
+        <v>-2.8744790000018838E-2</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">

</xml_diff>